<commit_message>
alterações para o segundo cenário
</commit_message>
<xml_diff>
--- a/Agendar servicos/17. Análise dos Eventos para cada Cenário.xlsx
+++ b/Agendar servicos/17. Análise dos Eventos para cada Cenário.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elton\Desktop\OPE\OPE_Artefatos_HAIR2U\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elton\Desktop\OPE\OPE_Artefatos_HAIR2U\Agendar servicos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB5FF260-90EA-4429-B6A6-0CE41BAEC034}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C738DBD9-A6D3-4BEF-B0E4-C80A24498DAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C877A977-5D9B-4F08-BA96-DC6508DF2181}"/>
+    <workbookView xWindow="-40365" yWindow="2970" windowWidth="18060" windowHeight="9180" xr2:uid="{C877A977-5D9B-4F08-BA96-DC6508DF2181}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>capacidade</t>
   </si>
@@ -82,13 +82,19 @@
   </si>
   <si>
     <t>X(2)</t>
+  </si>
+  <si>
+    <t>Receber serviços</t>
+  </si>
+  <si>
+    <t>Cliente informa que está agendado</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -99,6 +105,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="7"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -120,18 +134,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF0070C0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -148,8 +150,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -222,32 +236,52 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -259,9 +293,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="255" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -270,6 +301,69 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -656,10 +750,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6A3E32E-1996-41D2-AF64-2CDCA275956E}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -681,41 +775,41 @@
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="16"/>
-      <c r="G1" s="15" t="s">
+      <c r="F1" s="13"/>
+      <c r="G1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="17"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="6"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="4"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="12"/>
+      <c r="B2" s="10"/>
       <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="H2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="I2" s="9" t="s">
         <v>15</v>
       </c>
       <c r="J2" s="3" t="s">
@@ -723,65 +817,145 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="13"/>
-      <c r="B3" s="14" t="s">
+      <c r="A3" s="11"/>
+      <c r="B3" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="17">
         <v>1</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="8" t="s">
+      <c r="E3" s="5"/>
+      <c r="F3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="10"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="8"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="13"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="4">
+      <c r="A4" s="11"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="17">
         <v>2</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="7"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="10"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="8"/>
     </row>
     <row r="5" spans="1:10" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="13"/>
-      <c r="B5" s="5" t="s">
+      <c r="A5" s="11"/>
+      <c r="B5" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="17">
         <v>3</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="8" t="s">
+      <c r="E5" s="5"/>
+      <c r="F5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="10"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="8"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="19">
+        <v>4</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="20"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="22"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="34"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="26"/>
+      <c r="J7" s="27"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="34"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="27"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="34"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="27"/>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="35"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="31"/>
+      <c r="J10" s="32"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="15">
+    <mergeCell ref="C6:C10"/>
+    <mergeCell ref="D6:D10"/>
+    <mergeCell ref="J6:J10"/>
+    <mergeCell ref="I6:I10"/>
+    <mergeCell ref="H6:H10"/>
+    <mergeCell ref="G6:G10"/>
+    <mergeCell ref="F6:F10"/>
+    <mergeCell ref="E6:E10"/>
+    <mergeCell ref="A6:A10"/>
+    <mergeCell ref="B6:B10"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="B3:B4"/>

</xml_diff>